<commit_message>
Add column to dwglog2.db: dwg_index. WIP to addust dwglog2.py modified db
</commit_message>
<xml_diff>
--- a/dwglogdata2.xlsx
+++ b/dwglogdata2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="135">
   <si>
     <t xml:space="preserve">Drawing Number</t>
   </si>
@@ -419,6 +419,12 @@
   </si>
   <si>
     <t xml:space="preserve">11/6/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0018643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
   </si>
 </sst>
 </file>
@@ -527,8 +533,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1549,6 +1555,26 @@
         <v>132</v>
       </c>
       <c r="F54" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55" s="0" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>